<commit_message>
fixed memory leak issues. TODO: fix READY messages for multicast
</commit_message>
<xml_diff>
--- a/dataLog.xlsx
+++ b/dataLog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId2" state="visible"/>
@@ -15,6 +15,10 @@
     <sheet name="2024_6_3 13_31" sheetId="5" r:id="rId7"/>
     <sheet name="2024_6_3 13_35" sheetId="6" r:id="rId8"/>
     <sheet name="2024_6_3 13_36" sheetId="7" r:id="rId9"/>
+    <sheet name="2024_6_3 15_55" sheetId="8" r:id="rId10"/>
+    <sheet name="2024_6_3 15_56" sheetId="9" r:id="rId11"/>
+    <sheet name="2024_6_5 18_27" sheetId="10" r:id="rId12"/>
+    <sheet name="2024_6_10 16_6" sheetId="11" r:id="rId13"/>
   </sheets>
   <calcPr iterateCount="100" iterateDelta="0.001" refMode="A1"/>
   <extLst>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>UserCacheSize</t>
   </si>
@@ -261,6 +265,24 @@
   <si>
     <t>346 ms</t>
   </si>
+  <si>
+    <t>6020 ms</t>
+  </si>
+  <si>
+    <t>Another one was fetching first</t>
+  </si>
+  <si>
+    <t>30220 ms</t>
+  </si>
+  <si>
+    <t>45378 ms</t>
+  </si>
+  <si>
+    <t>60308 ms</t>
+  </si>
+  <si>
+    <t>150524 ms</t>
+  </si>
 </sst>
 </file>
 
@@ -376,6 +398,3220 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>333</v>
+      </c>
+      <c r="G4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="F5">
+        <v>334</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6">
+        <v>335</v>
+      </c>
+      <c r="G6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7">
+        <v>1003</v>
+      </c>
+      <c r="F7">
+        <v>336</v>
+      </c>
+      <c r="G7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8">
+        <v>2016</v>
+      </c>
+      <c r="F8">
+        <v>337</v>
+      </c>
+      <c r="G8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9">
+        <v>3017</v>
+      </c>
+      <c r="F9">
+        <v>338</v>
+      </c>
+      <c r="G9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10">
+        <v>3017</v>
+      </c>
+      <c r="F10">
+        <v>200</v>
+      </c>
+      <c r="G10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11">
+        <v>3009</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12">
+        <v>3008</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17">
+        <v>3015</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18">
+        <v>3029</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19">
+        <v>3027</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20">
+        <v>3020</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22">
+        <v>3045</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23">
+        <v>3040</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24">
+        <v>3053</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25">
+        <v>3013</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26">
+        <v>3013</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27">
+        <v>3013</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28">
+        <v>3033</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29">
+        <v>3033</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30">
+        <v>3025</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32">
+        <v>3006</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34">
+        <v>3008</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35">
+        <v>3009</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" t="s">
+        <v>69</v>
+      </c>
+      <c r="D36">
+        <v>3018</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37">
+        <v>3013</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>3</v>
+      </c>
+      <c r="B38" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" t="s">
+        <v>69</v>
+      </c>
+      <c r="D38">
+        <v>3018</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39">
+        <v>3010</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>3</v>
+      </c>
+      <c r="B41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41">
+        <v>3006</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42">
+        <v>3004</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" t="s">
+        <v>69</v>
+      </c>
+      <c r="D43">
+        <v>3013</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>3</v>
+      </c>
+      <c r="B44" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44">
+        <v>3018</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>2</v>
+      </c>
+      <c r="B45" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" t="s">
+        <v>69</v>
+      </c>
+      <c r="D45">
+        <v>3018</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46">
+        <v>3006</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>3</v>
+      </c>
+      <c r="B47" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>2</v>
+      </c>
+      <c r="B48" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" t="s">
+        <v>69</v>
+      </c>
+      <c r="D49">
+        <v>3023</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>3</v>
+      </c>
+      <c r="B50" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" t="s">
+        <v>69</v>
+      </c>
+      <c r="D50">
+        <v>3022</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>2</v>
+      </c>
+      <c r="B51" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51" t="s">
+        <v>69</v>
+      </c>
+      <c r="D51">
+        <v>3046</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" t="s">
+        <v>69</v>
+      </c>
+      <c r="D52">
+        <v>3024</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>3</v>
+      </c>
+      <c r="B53" t="s">
+        <v>36</v>
+      </c>
+      <c r="C53" t="s">
+        <v>69</v>
+      </c>
+      <c r="D53">
+        <v>3024</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
+        <v>2</v>
+      </c>
+      <c r="B54" t="s">
+        <v>28</v>
+      </c>
+      <c r="C54" t="s">
+        <v>69</v>
+      </c>
+      <c r="D54">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55" t="s">
+        <v>30</v>
+      </c>
+      <c r="C55" t="s">
+        <v>69</v>
+      </c>
+      <c r="D55">
+        <v>3007</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56">
+        <v>3</v>
+      </c>
+      <c r="B56" t="s">
+        <v>45</v>
+      </c>
+      <c r="C56" t="s">
+        <v>69</v>
+      </c>
+      <c r="D56">
+        <v>3010</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57">
+        <v>2</v>
+      </c>
+      <c r="B57" t="s">
+        <v>55</v>
+      </c>
+      <c r="C57" t="s">
+        <v>69</v>
+      </c>
+      <c r="D57">
+        <v>3011</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58" t="s">
+        <v>28</v>
+      </c>
+      <c r="C58" t="s">
+        <v>69</v>
+      </c>
+      <c r="D58">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59">
+        <v>3</v>
+      </c>
+      <c r="B59" t="s">
+        <v>21</v>
+      </c>
+      <c r="C59" t="s">
+        <v>69</v>
+      </c>
+      <c r="D59">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60">
+        <v>2</v>
+      </c>
+      <c r="B60" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60" t="s">
+        <v>69</v>
+      </c>
+      <c r="D60">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="B61" t="s">
+        <v>53</v>
+      </c>
+      <c r="C61" t="s">
+        <v>69</v>
+      </c>
+      <c r="D61">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62">
+        <v>3</v>
+      </c>
+      <c r="B62" t="s">
+        <v>18</v>
+      </c>
+      <c r="C62" t="s">
+        <v>69</v>
+      </c>
+      <c r="D62">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63">
+        <v>2</v>
+      </c>
+      <c r="B63" t="s">
+        <v>53</v>
+      </c>
+      <c r="C63" t="s">
+        <v>69</v>
+      </c>
+      <c r="D63">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64" t="s">
+        <v>14</v>
+      </c>
+      <c r="C64" t="s">
+        <v>69</v>
+      </c>
+      <c r="D64">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65">
+        <v>3</v>
+      </c>
+      <c r="B65" t="s">
+        <v>36</v>
+      </c>
+      <c r="C65" t="s">
+        <v>69</v>
+      </c>
+      <c r="D65">
+        <v>3018</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66">
+        <v>2</v>
+      </c>
+      <c r="B66" t="s">
+        <v>48</v>
+      </c>
+      <c r="C66" t="s">
+        <v>69</v>
+      </c>
+      <c r="D66">
+        <v>3020</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="true" workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>200</v>
+      </c>
+      <c r="G4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="F5">
+        <v>333</v>
+      </c>
+      <c r="G5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6">
+        <v>334</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7">
+        <v>1002</v>
+      </c>
+      <c r="F7">
+        <v>335</v>
+      </c>
+      <c r="G7" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8">
+        <v>3002</v>
+      </c>
+      <c r="F8">
+        <v>336</v>
+      </c>
+      <c r="G8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9">
+        <v>3002</v>
+      </c>
+      <c r="F9">
+        <v>337</v>
+      </c>
+      <c r="G9" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10">
+        <v>3001</v>
+      </c>
+      <c r="F10">
+        <v>338</v>
+      </c>
+      <c r="G10" t="s">
+        <v>79</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15">
+        <v>3007</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16">
+        <v>3006</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21">
+        <v>3019</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22">
+        <v>3020</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23">
+        <v>3020</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26">
+        <v>3007</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27">
+        <v>3009</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29">
+        <v>3009</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30">
+        <v>3007</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31">
+        <v>3019</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32">
+        <v>3018</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34">
+        <v>3007</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35">
+        <v>3008</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="B36" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" t="s">
+        <v>69</v>
+      </c>
+      <c r="D36">
+        <v>3007</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="B37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" t="s">
+        <v>69</v>
+      </c>
+      <c r="D38">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39">
+        <v>3006</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>3</v>
+      </c>
+      <c r="B40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40">
+        <v>3008</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41">
+        <v>3010</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42">
+        <v>3007</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>3</v>
+      </c>
+      <c r="B43" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" t="s">
+        <v>69</v>
+      </c>
+      <c r="D43">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>2</v>
+      </c>
+      <c r="B45" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" t="s">
+        <v>69</v>
+      </c>
+      <c r="D45">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>3</v>
+      </c>
+      <c r="B46" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46">
+        <v>3007</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47" t="s">
+        <v>42</v>
+      </c>
+      <c r="C47" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47">
+        <v>3007</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>2</v>
+      </c>
+      <c r="B48" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48">
+        <v>3006</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>3</v>
+      </c>
+      <c r="B49" t="s">
+        <v>23</v>
+      </c>
+      <c r="C49" t="s">
+        <v>69</v>
+      </c>
+      <c r="D49">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50" t="s">
+        <v>56</v>
+      </c>
+      <c r="C50" t="s">
+        <v>69</v>
+      </c>
+      <c r="D50">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>2</v>
+      </c>
+      <c r="B51" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" t="s">
+        <v>69</v>
+      </c>
+      <c r="D51">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>3</v>
+      </c>
+      <c r="B52" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" t="s">
+        <v>69</v>
+      </c>
+      <c r="D52">
+        <v>3006</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53" t="s">
+        <v>41</v>
+      </c>
+      <c r="C53" t="s">
+        <v>69</v>
+      </c>
+      <c r="D53">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
+        <v>2</v>
+      </c>
+      <c r="B54" t="s">
+        <v>26</v>
+      </c>
+      <c r="C54" t="s">
+        <v>69</v>
+      </c>
+      <c r="D54">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55">
+        <v>3</v>
+      </c>
+      <c r="B55" t="s">
+        <v>26</v>
+      </c>
+      <c r="C55" t="s">
+        <v>69</v>
+      </c>
+      <c r="D55">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56">
+        <v>1</v>
+      </c>
+      <c r="B56" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" t="s">
+        <v>69</v>
+      </c>
+      <c r="D56">
+        <v>3010</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57">
+        <v>2</v>
+      </c>
+      <c r="B57" t="s">
+        <v>45</v>
+      </c>
+      <c r="C57" t="s">
+        <v>69</v>
+      </c>
+      <c r="D57">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58">
+        <v>3</v>
+      </c>
+      <c r="B58" t="s">
+        <v>53</v>
+      </c>
+      <c r="C58" t="s">
+        <v>69</v>
+      </c>
+      <c r="D58">
+        <v>3023</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59" t="s">
+        <v>51</v>
+      </c>
+      <c r="C59" t="s">
+        <v>69</v>
+      </c>
+      <c r="D59">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60">
+        <v>2</v>
+      </c>
+      <c r="B60" t="s">
+        <v>29</v>
+      </c>
+      <c r="C60" t="s">
+        <v>69</v>
+      </c>
+      <c r="D60">
+        <v>3011</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61">
+        <v>3</v>
+      </c>
+      <c r="B61" t="s">
+        <v>56</v>
+      </c>
+      <c r="C61" t="s">
+        <v>69</v>
+      </c>
+      <c r="D61">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62" t="s">
+        <v>40</v>
+      </c>
+      <c r="C62" t="s">
+        <v>69</v>
+      </c>
+      <c r="D62">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63">
+        <v>2</v>
+      </c>
+      <c r="B63" t="s">
+        <v>32</v>
+      </c>
+      <c r="C63" t="s">
+        <v>69</v>
+      </c>
+      <c r="D63">
+        <v>3015</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64">
+        <v>3</v>
+      </c>
+      <c r="B64" t="s">
+        <v>61</v>
+      </c>
+      <c r="C64" t="s">
+        <v>69</v>
+      </c>
+      <c r="D64">
+        <v>3007</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65">
+        <v>1</v>
+      </c>
+      <c r="B65" t="s">
+        <v>32</v>
+      </c>
+      <c r="C65" t="s">
+        <v>69</v>
+      </c>
+      <c r="D65">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66">
+        <v>2</v>
+      </c>
+      <c r="B66" t="s">
+        <v>61</v>
+      </c>
+      <c r="C66" t="s">
+        <v>69</v>
+      </c>
+      <c r="D66">
+        <v>3017</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67">
+        <v>3</v>
+      </c>
+      <c r="B67" t="s">
+        <v>36</v>
+      </c>
+      <c r="C67" t="s">
+        <v>69</v>
+      </c>
+      <c r="D67">
+        <v>3108</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68">
+        <v>1</v>
+      </c>
+      <c r="B68" t="s">
+        <v>59</v>
+      </c>
+      <c r="C68" t="s">
+        <v>69</v>
+      </c>
+      <c r="D68">
+        <v>3116</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69">
+        <v>2</v>
+      </c>
+      <c r="B69" t="s">
+        <v>57</v>
+      </c>
+      <c r="C69" t="s">
+        <v>69</v>
+      </c>
+      <c r="D69">
+        <v>3130</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70">
+        <v>3</v>
+      </c>
+      <c r="B70" t="s">
+        <v>33</v>
+      </c>
+      <c r="C70" t="s">
+        <v>69</v>
+      </c>
+      <c r="D70">
+        <v>3038</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71">
+        <v>1</v>
+      </c>
+      <c r="B71" t="s">
+        <v>15</v>
+      </c>
+      <c r="C71" t="s">
+        <v>69</v>
+      </c>
+      <c r="D71">
+        <v>3038</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72">
+        <v>2</v>
+      </c>
+      <c r="B72" t="s">
+        <v>15</v>
+      </c>
+      <c r="C72" t="s">
+        <v>69</v>
+      </c>
+      <c r="D72">
+        <v>3011</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73">
+        <v>3</v>
+      </c>
+      <c r="B73" t="s">
+        <v>44</v>
+      </c>
+      <c r="C73" t="s">
+        <v>69</v>
+      </c>
+      <c r="D73">
+        <v>3011</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74">
+        <v>1</v>
+      </c>
+      <c r="B74" t="s">
+        <v>55</v>
+      </c>
+      <c r="C74" t="s">
+        <v>69</v>
+      </c>
+      <c r="D74">
+        <v>3025</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75">
+        <v>2</v>
+      </c>
+      <c r="B75" t="s">
+        <v>23</v>
+      </c>
+      <c r="C75" t="s">
+        <v>69</v>
+      </c>
+      <c r="D75">
+        <v>3034</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76">
+        <v>3</v>
+      </c>
+      <c r="B76" t="s">
+        <v>46</v>
+      </c>
+      <c r="C76" t="s">
+        <v>69</v>
+      </c>
+      <c r="D76">
+        <v>3043</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77">
+        <v>1</v>
+      </c>
+      <c r="B77" t="s">
+        <v>28</v>
+      </c>
+      <c r="C77" t="s">
+        <v>69</v>
+      </c>
+      <c r="D77">
+        <v>3022</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78">
+        <v>2</v>
+      </c>
+      <c r="B78" t="s">
+        <v>27</v>
+      </c>
+      <c r="C78" t="s">
+        <v>69</v>
+      </c>
+      <c r="D78">
+        <v>3010</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79">
+        <v>3</v>
+      </c>
+      <c r="B79" t="s">
+        <v>35</v>
+      </c>
+      <c r="C79" t="s">
+        <v>69</v>
+      </c>
+      <c r="D79">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80">
+        <v>1</v>
+      </c>
+      <c r="B80" t="s">
+        <v>41</v>
+      </c>
+      <c r="C80" t="s">
+        <v>69</v>
+      </c>
+      <c r="D80">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81">
+        <v>2</v>
+      </c>
+      <c r="B81" t="s">
+        <v>28</v>
+      </c>
+      <c r="C81" t="s">
+        <v>69</v>
+      </c>
+      <c r="D81">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82">
+        <v>3</v>
+      </c>
+      <c r="B82" t="s">
+        <v>26</v>
+      </c>
+      <c r="C82" t="s">
+        <v>69</v>
+      </c>
+      <c r="D82">
+        <v>3007</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83">
+        <v>1</v>
+      </c>
+      <c r="B83" t="s">
+        <v>32</v>
+      </c>
+      <c r="C83" t="s">
+        <v>69</v>
+      </c>
+      <c r="D83">
+        <v>3008</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84">
+        <v>2</v>
+      </c>
+      <c r="B84" t="s">
+        <v>56</v>
+      </c>
+      <c r="C84" t="s">
+        <v>69</v>
+      </c>
+      <c r="D84">
+        <v>3006</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85">
+        <v>3</v>
+      </c>
+      <c r="B85" t="s">
+        <v>24</v>
+      </c>
+      <c r="C85" t="s">
+        <v>69</v>
+      </c>
+      <c r="D85">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86">
+        <v>1</v>
+      </c>
+      <c r="B86" t="s">
+        <v>23</v>
+      </c>
+      <c r="C86" t="s">
+        <v>69</v>
+      </c>
+      <c r="D86">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87">
+        <v>2</v>
+      </c>
+      <c r="B87" t="s">
+        <v>43</v>
+      </c>
+      <c r="C87" t="s">
+        <v>69</v>
+      </c>
+      <c r="D87">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88">
+        <v>3</v>
+      </c>
+      <c r="B88" t="s">
+        <v>43</v>
+      </c>
+      <c r="C88" t="s">
+        <v>69</v>
+      </c>
+      <c r="D88">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89">
+        <v>1</v>
+      </c>
+      <c r="B89" t="s">
+        <v>14</v>
+      </c>
+      <c r="C89" t="s">
+        <v>69</v>
+      </c>
+      <c r="D89">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90">
+        <v>2</v>
+      </c>
+      <c r="B90" t="s">
+        <v>54</v>
+      </c>
+      <c r="C90" t="s">
+        <v>69</v>
+      </c>
+      <c r="D90">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91">
+        <v>3</v>
+      </c>
+      <c r="B91" t="s">
+        <v>26</v>
+      </c>
+      <c r="C91" t="s">
+        <v>69</v>
+      </c>
+      <c r="D91">
+        <v>3006</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92">
+        <v>1</v>
+      </c>
+      <c r="B92" t="s">
+        <v>30</v>
+      </c>
+      <c r="C92" t="s">
+        <v>69</v>
+      </c>
+      <c r="D92">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93">
+        <v>2</v>
+      </c>
+      <c r="B93" t="s">
+        <v>16</v>
+      </c>
+      <c r="C93" t="s">
+        <v>69</v>
+      </c>
+      <c r="D93">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94">
+        <v>3</v>
+      </c>
+      <c r="B94" t="s">
+        <v>40</v>
+      </c>
+      <c r="C94" t="s">
+        <v>69</v>
+      </c>
+      <c r="D94">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95">
+        <v>1</v>
+      </c>
+      <c r="B95" t="s">
+        <v>14</v>
+      </c>
+      <c r="C95" t="s">
+        <v>69</v>
+      </c>
+      <c r="D95">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96">
+        <v>2</v>
+      </c>
+      <c r="B96" t="s">
+        <v>33</v>
+      </c>
+      <c r="C96" t="s">
+        <v>69</v>
+      </c>
+      <c r="D96">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97">
+        <v>3</v>
+      </c>
+      <c r="B97" t="s">
+        <v>56</v>
+      </c>
+      <c r="C97" t="s">
+        <v>69</v>
+      </c>
+      <c r="D97">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98">
+        <v>1</v>
+      </c>
+      <c r="B98" t="s">
+        <v>34</v>
+      </c>
+      <c r="C98" t="s">
+        <v>69</v>
+      </c>
+      <c r="D98">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99">
+        <v>2</v>
+      </c>
+      <c r="B99" t="s">
+        <v>62</v>
+      </c>
+      <c r="C99" t="s">
+        <v>69</v>
+      </c>
+      <c r="D99">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100">
+        <v>3</v>
+      </c>
+      <c r="B100" t="s">
+        <v>34</v>
+      </c>
+      <c r="C100" t="s">
+        <v>69</v>
+      </c>
+      <c r="D100">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101">
+        <v>1</v>
+      </c>
+      <c r="B101" t="s">
+        <v>54</v>
+      </c>
+      <c r="C101" t="s">
+        <v>69</v>
+      </c>
+      <c r="D101">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102">
+        <v>2</v>
+      </c>
+      <c r="B102" t="s">
+        <v>23</v>
+      </c>
+      <c r="C102" t="s">
+        <v>69</v>
+      </c>
+      <c r="D102">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103">
+        <v>3</v>
+      </c>
+      <c r="B103" t="s">
+        <v>56</v>
+      </c>
+      <c r="C103" t="s">
+        <v>69</v>
+      </c>
+      <c r="D103">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104">
+        <v>1</v>
+      </c>
+      <c r="B104" t="s">
+        <v>33</v>
+      </c>
+      <c r="C104" t="s">
+        <v>69</v>
+      </c>
+      <c r="D104">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105">
+        <v>2</v>
+      </c>
+      <c r="B105" t="s">
+        <v>32</v>
+      </c>
+      <c r="C105" t="s">
+        <v>69</v>
+      </c>
+      <c r="D105">
+        <v>3007</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106">
+        <v>3</v>
+      </c>
+      <c r="B106" t="s">
+        <v>41</v>
+      </c>
+      <c r="C106" t="s">
+        <v>69</v>
+      </c>
+      <c r="D106">
+        <v>3026</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107">
+        <v>1</v>
+      </c>
+      <c r="B107" t="s">
+        <v>28</v>
+      </c>
+      <c r="C107" t="s">
+        <v>69</v>
+      </c>
+      <c r="D107">
+        <v>3029</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108">
+        <v>2</v>
+      </c>
+      <c r="B108" t="s">
+        <v>38</v>
+      </c>
+      <c r="C108" t="s">
+        <v>69</v>
+      </c>
+      <c r="D108">
+        <v>3029</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109">
+        <v>3</v>
+      </c>
+      <c r="B109" t="s">
+        <v>49</v>
+      </c>
+      <c r="C109" t="s">
+        <v>69</v>
+      </c>
+      <c r="D109">
+        <v>3008</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110">
+        <v>1</v>
+      </c>
+      <c r="B110" t="s">
+        <v>45</v>
+      </c>
+      <c r="C110" t="s">
+        <v>69</v>
+      </c>
+      <c r="D110">
+        <v>3004</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111">
+        <v>2</v>
+      </c>
+      <c r="B111" t="s">
+        <v>49</v>
+      </c>
+      <c r="C111" t="s">
+        <v>69</v>
+      </c>
+      <c r="D111">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112">
+        <v>3</v>
+      </c>
+      <c r="B112" t="s">
+        <v>34</v>
+      </c>
+      <c r="C112" t="s">
+        <v>69</v>
+      </c>
+      <c r="D112">
+        <v>3004</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113">
+        <v>1</v>
+      </c>
+      <c r="B113" t="s">
+        <v>48</v>
+      </c>
+      <c r="C113" t="s">
+        <v>69</v>
+      </c>
+      <c r="D113">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114">
+        <v>2</v>
+      </c>
+      <c r="B114" t="s">
+        <v>35</v>
+      </c>
+      <c r="C114" t="s">
+        <v>69</v>
+      </c>
+      <c r="D114">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115">
+        <v>3</v>
+      </c>
+      <c r="B115" t="s">
+        <v>26</v>
+      </c>
+      <c r="C115" t="s">
+        <v>69</v>
+      </c>
+      <c r="D115">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116">
+        <v>1</v>
+      </c>
+      <c r="B116" t="s">
+        <v>17</v>
+      </c>
+      <c r="C116" t="s">
+        <v>69</v>
+      </c>
+      <c r="D116">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117">
+        <v>2</v>
+      </c>
+      <c r="B117" t="s">
+        <v>23</v>
+      </c>
+      <c r="C117" t="s">
+        <v>69</v>
+      </c>
+      <c r="D117">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118">
+        <v>3</v>
+      </c>
+      <c r="B118" t="s">
+        <v>12</v>
+      </c>
+      <c r="C118" t="s">
+        <v>69</v>
+      </c>
+      <c r="D118">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119">
+        <v>1</v>
+      </c>
+      <c r="B119" t="s">
+        <v>24</v>
+      </c>
+      <c r="C119" t="s">
+        <v>69</v>
+      </c>
+      <c r="D119">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120">
+        <v>2</v>
+      </c>
+      <c r="B120" t="s">
+        <v>50</v>
+      </c>
+      <c r="C120" t="s">
+        <v>69</v>
+      </c>
+      <c r="D120">
+        <v>3009</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121">
+        <v>3</v>
+      </c>
+      <c r="B121" t="s">
+        <v>48</v>
+      </c>
+      <c r="C121" t="s">
+        <v>69</v>
+      </c>
+      <c r="D121">
+        <v>3008</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122">
+        <v>1</v>
+      </c>
+      <c r="B122" t="s">
+        <v>42</v>
+      </c>
+      <c r="C122" t="s">
+        <v>69</v>
+      </c>
+      <c r="D122">
+        <v>3008</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123">
+        <v>2</v>
+      </c>
+      <c r="B123" t="s">
+        <v>43</v>
+      </c>
+      <c r="C123" t="s">
+        <v>69</v>
+      </c>
+      <c r="D123">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124">
+        <v>3</v>
+      </c>
+      <c r="B124" t="s">
+        <v>50</v>
+      </c>
+      <c r="C124" t="s">
+        <v>69</v>
+      </c>
+      <c r="D124">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125">
+        <v>1</v>
+      </c>
+      <c r="B125" t="s">
+        <v>14</v>
+      </c>
+      <c r="C125" t="s">
+        <v>69</v>
+      </c>
+      <c r="D125">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126">
+        <v>2</v>
+      </c>
+      <c r="B126" t="s">
+        <v>59</v>
+      </c>
+      <c r="C126" t="s">
+        <v>69</v>
+      </c>
+      <c r="D126">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127">
+        <v>3</v>
+      </c>
+      <c r="B127" t="s">
+        <v>42</v>
+      </c>
+      <c r="C127" t="s">
+        <v>69</v>
+      </c>
+      <c r="D127">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128">
+        <v>1</v>
+      </c>
+      <c r="B128" t="s">
+        <v>30</v>
+      </c>
+      <c r="C128" t="s">
+        <v>69</v>
+      </c>
+      <c r="D128">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129">
+        <v>2</v>
+      </c>
+      <c r="B129" t="s">
+        <v>12</v>
+      </c>
+      <c r="C129" t="s">
+        <v>69</v>
+      </c>
+      <c r="D129">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130">
+        <v>3</v>
+      </c>
+      <c r="B130" t="s">
+        <v>32</v>
+      </c>
+      <c r="C130" t="s">
+        <v>69</v>
+      </c>
+      <c r="D130">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131">
+        <v>1</v>
+      </c>
+      <c r="B131" t="s">
+        <v>45</v>
+      </c>
+      <c r="C131" t="s">
+        <v>69</v>
+      </c>
+      <c r="D131">
+        <v>3004</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132">
+        <v>2</v>
+      </c>
+      <c r="B132" t="s">
+        <v>34</v>
+      </c>
+      <c r="C132" t="s">
+        <v>69</v>
+      </c>
+      <c r="D132">
+        <v>3004</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133">
+        <v>3</v>
+      </c>
+      <c r="B133" t="s">
+        <v>42</v>
+      </c>
+      <c r="C133" t="s">
+        <v>69</v>
+      </c>
+      <c r="D133">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134">
+        <v>1</v>
+      </c>
+      <c r="B134" t="s">
+        <v>25</v>
+      </c>
+      <c r="C134" t="s">
+        <v>69</v>
+      </c>
+      <c r="D134">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135">
+        <v>2</v>
+      </c>
+      <c r="B135" t="s">
+        <v>42</v>
+      </c>
+      <c r="C135" t="s">
+        <v>69</v>
+      </c>
+      <c r="D135">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136">
+        <v>3</v>
+      </c>
+      <c r="B136" t="s">
+        <v>29</v>
+      </c>
+      <c r="C136" t="s">
+        <v>69</v>
+      </c>
+      <c r="D136">
+        <v>3007</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137">
+        <v>1</v>
+      </c>
+      <c r="B137" t="s">
+        <v>35</v>
+      </c>
+      <c r="C137" t="s">
+        <v>69</v>
+      </c>
+      <c r="D137">
+        <v>3020</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138">
+        <v>2</v>
+      </c>
+      <c r="B138" t="s">
+        <v>24</v>
+      </c>
+      <c r="C138" t="s">
+        <v>69</v>
+      </c>
+      <c r="D138">
+        <v>3036</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139">
+        <v>3</v>
+      </c>
+      <c r="B139" t="s">
+        <v>18</v>
+      </c>
+      <c r="C139" t="s">
+        <v>69</v>
+      </c>
+      <c r="D139">
+        <v>3029</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140">
+        <v>1</v>
+      </c>
+      <c r="B140" t="s">
+        <v>15</v>
+      </c>
+      <c r="C140" t="s">
+        <v>69</v>
+      </c>
+      <c r="D140">
+        <v>3018</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141">
+        <v>2</v>
+      </c>
+      <c r="B141" t="s">
+        <v>60</v>
+      </c>
+      <c r="C141" t="s">
+        <v>69</v>
+      </c>
+      <c r="D141">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142">
+        <v>3</v>
+      </c>
+      <c r="B142" t="s">
+        <v>18</v>
+      </c>
+      <c r="C142" t="s">
+        <v>69</v>
+      </c>
+      <c r="D142">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143">
+        <v>1</v>
+      </c>
+      <c r="B143" t="s">
+        <v>43</v>
+      </c>
+      <c r="C143" t="s">
+        <v>69</v>
+      </c>
+      <c r="D143">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144">
+        <v>2</v>
+      </c>
+      <c r="B144" t="s">
+        <v>50</v>
+      </c>
+      <c r="C144" t="s">
+        <v>69</v>
+      </c>
+      <c r="D144">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145">
+        <v>3</v>
+      </c>
+      <c r="B145" t="s">
+        <v>55</v>
+      </c>
+      <c r="C145" t="s">
+        <v>69</v>
+      </c>
+      <c r="D145">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146">
+        <v>1</v>
+      </c>
+      <c r="B146" t="s">
+        <v>22</v>
+      </c>
+      <c r="C146" t="s">
+        <v>69</v>
+      </c>
+      <c r="D146">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147">
+        <v>2</v>
+      </c>
+      <c r="B147" t="s">
+        <v>37</v>
+      </c>
+      <c r="C147" t="s">
+        <v>69</v>
+      </c>
+      <c r="D147">
+        <v>3006</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148">
+        <v>3</v>
+      </c>
+      <c r="B148" t="s">
+        <v>41</v>
+      </c>
+      <c r="C148" t="s">
+        <v>69</v>
+      </c>
+      <c r="D148">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149">
+        <v>1</v>
+      </c>
+      <c r="B149" t="s">
+        <v>57</v>
+      </c>
+      <c r="C149" t="s">
+        <v>69</v>
+      </c>
+      <c r="D149">
+        <v>3006</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150">
+        <v>2</v>
+      </c>
+      <c r="B150" t="s">
+        <v>12</v>
+      </c>
+      <c r="C150" t="s">
+        <v>69</v>
+      </c>
+      <c r="D150">
+        <v>3013</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151">
+        <v>3</v>
+      </c>
+      <c r="B151" t="s">
+        <v>16</v>
+      </c>
+      <c r="C151" t="s">
+        <v>69</v>
+      </c>
+      <c r="D151">
+        <v>3013</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152">
+        <v>1</v>
+      </c>
+      <c r="B152" t="s">
+        <v>14</v>
+      </c>
+      <c r="C152" t="s">
+        <v>69</v>
+      </c>
+      <c r="D152">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153">
+        <v>2</v>
+      </c>
+      <c r="B153" t="s">
+        <v>24</v>
+      </c>
+      <c r="C153" t="s">
+        <v>69</v>
+      </c>
+      <c r="D153">
+        <v>3004</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154">
+        <v>3</v>
+      </c>
+      <c r="B154" t="s">
+        <v>35</v>
+      </c>
+      <c r="C154" t="s">
+        <v>69</v>
+      </c>
+      <c r="D154">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155">
+        <v>1</v>
+      </c>
+      <c r="B155" t="s">
+        <v>18</v>
+      </c>
+      <c r="C155" t="s">
+        <v>69</v>
+      </c>
+      <c r="D155">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156">
+        <v>2</v>
+      </c>
+      <c r="B156" t="s">
+        <v>46</v>
+      </c>
+      <c r="C156" t="s">
+        <v>69</v>
+      </c>
+      <c r="D156">
+        <v>3003</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
@@ -70993,7 +74229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -85115,4 +88351,992 @@
     </row>
   </sheetData>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>335</v>
+      </c>
+      <c r="G4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="F5">
+        <v>336</v>
+      </c>
+      <c r="G5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6">
+        <v>337</v>
+      </c>
+      <c r="G6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7">
+        <v>1004</v>
+      </c>
+      <c r="F7">
+        <v>338</v>
+      </c>
+      <c r="G7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8">
+        <v>2012</v>
+      </c>
+      <c r="F8">
+        <v>200</v>
+      </c>
+      <c r="G8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9">
+        <v>3013</v>
+      </c>
+      <c r="F9">
+        <v>333</v>
+      </c>
+      <c r="G9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10">
+        <v>3012</v>
+      </c>
+      <c r="F10">
+        <v>334</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11">
+        <v>3007</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12">
+        <v>3006</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>334</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="F5">
+        <v>335</v>
+      </c>
+      <c r="G5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6">
+        <v>336</v>
+      </c>
+      <c r="G6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7">
+        <v>1005</v>
+      </c>
+      <c r="F7">
+        <v>337</v>
+      </c>
+      <c r="G7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8">
+        <v>3005</v>
+      </c>
+      <c r="F8">
+        <v>338</v>
+      </c>
+      <c r="G8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9">
+        <v>3005</v>
+      </c>
+      <c r="F9">
+        <v>200</v>
+      </c>
+      <c r="G9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10">
+        <v>3001</v>
+      </c>
+      <c r="F10">
+        <v>333</v>
+      </c>
+      <c r="G10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12">
+        <v>3004</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13">
+        <v>3046</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14">
+        <v>3046</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15">
+        <v>3058</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18">
+        <v>3008</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19">
+        <v>3132</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20">
+        <v>3150</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21">
+        <v>3146</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22">
+        <v>3022</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23">
+        <v>3009</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24">
+        <v>3009</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27">
+        <v>3013</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28">
+        <v>3008</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29">
+        <v>3007</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30">
+        <v>3006</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31">
+        <v>3026</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32">
+        <v>3022</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33">
+        <v>3028</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34">
+        <v>3006</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>2</v>
+      </c>
+      <c r="B35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35">
+        <v>3007</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>3</v>
+      </c>
+      <c r="B36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" t="s">
+        <v>69</v>
+      </c>
+      <c r="D36">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" t="s">
+        <v>69</v>
+      </c>
+      <c r="D38">
+        <v>3006</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39">
+        <v>3008</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40">
+        <v>3008</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>2</v>
+      </c>
+      <c r="B41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>3</v>
+      </c>
+      <c r="B42" t="s">
+        <v>30</v>
+      </c>
+      <c r="C42" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42">
+        <v>3004</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" t="s">
+        <v>69</v>
+      </c>
+      <c r="D43">
+        <v>3007</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>2</v>
+      </c>
+      <c r="B44" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" t="s">
+        <v>69</v>
+      </c>
+      <c r="D45">
+        <v>3015</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46">
+        <v>3011</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>2</v>
+      </c>
+      <c r="B47" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47">
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>3</v>
+      </c>
+      <c r="B48" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48">
+        <v>3067</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>35</v>
+      </c>
+      <c r="C49" t="s">
+        <v>69</v>
+      </c>
+      <c r="D49">
+        <v>3067</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="B50" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" t="s">
+        <v>69</v>
+      </c>
+      <c r="D50">
+        <v>3009</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>3</v>
+      </c>
+      <c r="B51" t="s">
+        <v>35</v>
+      </c>
+      <c r="C51" t="s">
+        <v>69</v>
+      </c>
+      <c r="D51">
+        <v>3000</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>